<commit_message>
Bugfix nuts and allergens search exports
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/ExportAllergens.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/ExportAllergens.xlsx
@@ -16,6 +16,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Allergènes!$B$3:$AJ$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Allergènes!$B$3:$AJ$3</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Allergènes!$B$3:$AJ$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Allergènes!$B$3:$AJ$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Allergènes!$B$3:$AJ$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,7 +34,7 @@
     <t xml:space="preserve">TYPE</t>
   </si>
   <si>
-    <t xml:space="preserve">bcpg:finishedProduct</t>
+    <t xml:space="preserve">bcpg:product</t>
   </si>
   <si>
     <t xml:space="preserve">COLUMNS</t>
@@ -59,88 +61,88 @@
     <t xml:space="preserve">bcpg:legalName</t>
   </si>
   <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX1"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX1"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX2"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX2"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX3"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX3"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX4"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX4"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX5"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX5"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX6"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX6"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX7"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX7"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX8"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX8"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX9"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX9"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX10"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX10"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX11"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX11"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX12"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX12"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX13"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX13"]_bcpg:allergenListInVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX14"]_bcpg:allergenListVoluntary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "FX14"]_bcpg:allergenListInVoluntary</t>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AW"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AW"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AC"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AC"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AE"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AE"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AP"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AP"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AY"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AY"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AM"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AM"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AN"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AN"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AF"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AF"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "BC"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "BC"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "BM"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "BM"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AS"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AS"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AU"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "AU"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "NL"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "NL"]_bcpg:allergenListInVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "UM"]_bcpg:allergenListVoluntary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:allergenList[bcpg:allergenListAllergen#bcpg:allergenCode == "UM"]_bcpg:allergenListInVoluntary</t>
   </si>
   <si>
     <t xml:space="preserve">#</t>
@@ -395,16 +397,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <name val="Arial"/>
-        <charset val="1"/>
-        <family val="2"/>
-        <color rgb="FFFF3333"/>
-      </font>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -481,21 +473,21 @@
   <dimension ref="A1:AW3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J20" activeCellId="0" sqref="J20"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.3724489795918"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="36" min="9" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="36" min="9" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>